<commit_message>
Cleaned, created table into the database and loaded the labour-market  file into my database.
</commit_message>
<xml_diff>
--- a/LondonDataProject/data/raw/labour-market.xlsx
+++ b/LondonDataProject/data/raw/labour-market.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahamadoucamara/Documents/learning-data-engineering/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahamadoucamara/Documents/Analysis-Of-London-Public-Transportation-System-And-Its-Impact-On-Economic-And-Social/LondonDataProject/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D121BF-B4E1-6242-9A7E-612A612E9B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4E9135-26AE-A643-AE42-5B59241357D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20720" windowHeight="13280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>